<commit_message>
new rev 3 Gerbers, PDF, renders, BoM
</commit_message>
<xml_diff>
--- a/kicad/ClockIOT_PCB_specification.xlsx
+++ b/kicad/ClockIOT_PCB_specification.xlsx
@@ -46,7 +46,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">ClockIOT</t>
+    <t xml:space="preserve">ClockIOT rev 3</t>
   </si>
   <si>
     <r>
@@ -1014,14 +1014,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3643724696356"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.7935222672065"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8825910931174"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.02834008097166"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3684210526316"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.3076923076923"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.2267206477733"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.9676113360324"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.3643724696356"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.165991902834"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.7368421052632"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.5101214574899"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.8259109311741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1274,17 +1274,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="32.2226720647773"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="17.8259109311741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.9352226720648"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3684210526316"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.3684210526316"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="13.1983805668016"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="19.1943319838057"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="22.1093117408907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="21.165991902834"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="26.7368421052632"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="24.9392712550607"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.0566801619433"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
rev 4, added 3 pin headers for CLK/DAT/GND for building bigger matrices
</commit_message>
<xml_diff>
--- a/kicad/ClockIOT_PCB_specification.xlsx
+++ b/kicad/ClockIOT_PCB_specification.xlsx
@@ -46,7 +46,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">ClockIOT rev 3</t>
+    <t xml:space="preserve">ClockIOT rev 4</t>
   </si>
   <si>
     <r>
@@ -1014,14 +1014,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.3643724696356"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.165991902834"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.2834008097166"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.7368421052632"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.5101214574899"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.8259109311741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.3076923076923"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.1902834008097"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5384615384615"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.54251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.336032388664"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="12.6842105263158"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1274,17 +1274,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="13.1983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="19.1943319838057"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="22.1093117408907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="21.165991902834"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="26.7368421052632"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="24.9392712550607"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.7368421052632"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="23.7368421052632"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="28.7935222672065"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="26.8218623481781"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.2226720647773"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.9109311740891"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>